<commit_message>
UI Validations added V.51
</commit_message>
<xml_diff>
--- a/Test_Planner/VIAX_OrderCreation.xlsx
+++ b/Test_Planner/VIAX_OrderCreation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\Test_Planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AEED4C2-1992-4C98-B98F-FA189FCCB962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DB87D2-9D61-461A-9D05-54ACC0DCAF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3F52AFC6-D99D-4450-AD0F-1227D9226E9B}"/>
   </bookViews>
@@ -412,7 +412,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -784,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34CF3798-65B8-4491-99A4-6813C24FCF65}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -991,13 +991,13 @@
         <v>4</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12">
-        <v>5409448</v>
+        <v>50</v>
+      </c>
+      <c r="D12" s="13">
+        <v>5409419</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -1008,13 +1008,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D13" s="13">
-        <v>5409419</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>18</v>
+        <v>5409420</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -1025,13 +1025,13 @@
         <v>4</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D14" s="13">
-        <v>5409420</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>19</v>
+        <v>5409421</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -1042,13 +1042,13 @@
         <v>4</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D15" s="13">
-        <v>5409421</v>
+        <v>5409422</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -1059,13 +1059,13 @@
         <v>4</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D16" s="13">
-        <v>5409422</v>
+        <v>5409423</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -1076,13 +1076,13 @@
         <v>4</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D17" s="13">
-        <v>5409423</v>
+        <v>5409424</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -1093,13 +1093,13 @@
         <v>4</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D18" s="13">
-        <v>5409424</v>
+        <v>5409425</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -1110,13 +1110,13 @@
         <v>4</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D19" s="13">
-        <v>5409425</v>
+        <v>5409426</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -1127,13 +1127,13 @@
         <v>4</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D20" s="13">
-        <v>5409426</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>25</v>
+        <v>5409427</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1144,13 +1144,13 @@
         <v>4</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D21" s="13">
-        <v>5409427</v>
+        <v>5409428</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1161,13 +1161,13 @@
         <v>4</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D22" s="13">
-        <v>5409428</v>
+        <v>5409429</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1178,13 +1178,13 @@
         <v>4</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D23" s="13">
-        <v>5409429</v>
+        <v>5409430</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1195,13 +1195,13 @@
         <v>4</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D24" s="13">
-        <v>5409430</v>
+        <v>5409431</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1212,13 +1212,13 @@
         <v>4</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D25" s="13">
-        <v>5409431</v>
+        <v>5409432</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1229,13 +1229,13 @@
         <v>4</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D26" s="13">
-        <v>5409432</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>31</v>
+        <v>5409433</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -1246,13 +1246,13 @@
         <v>4</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D27" s="13">
-        <v>5409433</v>
+        <v>5409434</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -1263,13 +1263,13 @@
         <v>4</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D28" s="13">
-        <v>5409434</v>
+        <v>5409435</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1280,13 +1280,13 @@
         <v>4</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D29" s="13">
-        <v>5409435</v>
+        <v>5409436</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -1297,13 +1297,13 @@
         <v>4</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D30" s="13">
-        <v>5409436</v>
+        <v>5409437</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -1314,13 +1314,13 @@
         <v>4</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D31" s="13">
-        <v>5409437</v>
+        <v>5409438</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -1331,13 +1331,13 @@
         <v>4</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D32" s="13">
-        <v>5409438</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>37</v>
+        <v>5409439</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -1348,13 +1348,13 @@
         <v>4</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D33" s="13">
-        <v>5409439</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>38</v>
+        <v>49</v>
+      </c>
+      <c r="D33">
+        <v>5409448</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1374,21 +1374,21 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
     <cfRule type="expression" dxfId="2" priority="3641">
-      <formula>COUNTIF(G$55:G$100,#REF!)</formula>
+      <formula>COUNTIF(G$54:G$99,#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C34:E1048576 E3:E11 D12:E33">
-    <cfRule type="expression" dxfId="0" priority="3573">
+  <conditionalFormatting sqref="E3:E11 C33:E1048576 D12:E33">
+    <cfRule type="expression" dxfId="1" priority="3573">
       <formula>COUNTIF(#REF!,#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="expression" dxfId="1" priority="3642">
+    <cfRule type="expression" dxfId="0" priority="3642">
       <formula>COUNTIF(#REF!,#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B33" xr:uid="{DE21EE38-54D7-44B6-A9E8-B480FE2F7BC6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B11 B12:B33" xr:uid="{DE21EE38-54D7-44B6-A9E8-B480FE2F7BC6}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1601,18 +1601,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1635,14 +1635,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9A5492E-A32A-41EE-AAEE-6E8BE77D7028}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34FB7BFF-CBF3-491F-A454-15CC4708CCB1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -1657,4 +1649,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9A5492E-A32A-41EE-AAEE-6E8BE77D7028}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
UI Validations added V.57
</commit_message>
<xml_diff>
--- a/Test_Planner/VIAX_OrderCreation.xlsx
+++ b/Test_Planner/VIAX_OrderCreation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\Test_Planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DB87D2-9D61-461A-9D05-54ACC0DCAF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C275AFB9-5394-4247-A24D-E37FB7606695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3F52AFC6-D99D-4450-AD0F-1227D9226E9B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="75">
   <si>
     <t>SuteName</t>
   </si>
@@ -251,6 +251,18 @@
   </si>
   <si>
     <t>CO_NW_32</t>
+  </si>
+  <si>
+    <t>CO_NW_33</t>
+  </si>
+  <si>
+    <t>CO_NW_34</t>
+  </si>
+  <si>
+    <t>Validate the Order Status in DBS</t>
+  </si>
+  <si>
+    <t>SAPValidations</t>
   </si>
 </sst>
 </file>
@@ -394,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -413,6 +425,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -782,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34CF3798-65B8-4491-99A4-6813C24FCF65}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1355,6 +1368,40 @@
       </c>
       <c r="E33" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34">
+        <v>5411316</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35">
+        <v>5411317</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1377,7 +1424,7 @@
       <formula>COUNTIF(G$54:G$99,#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E11 C33:E1048576 D12:E33">
+  <conditionalFormatting sqref="E3:E11 D12:E33 C33:E1048576">
     <cfRule type="expression" dxfId="1" priority="3573">
       <formula>COUNTIF(#REF!,#REF!)</formula>
     </cfRule>
@@ -1388,7 +1435,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B11 B12:B33" xr:uid="{DE21EE38-54D7-44B6-A9E8-B480FE2F7BC6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B35" xr:uid="{DE21EE38-54D7-44B6-A9E8-B480FE2F7BC6}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1601,18 +1648,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1635,6 +1682,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9A5492E-A32A-41EE-AAEE-6E8BE77D7028}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34FB7BFF-CBF3-491F-A454-15CC4708CCB1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -1649,12 +1704,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9A5492E-A32A-41EE-AAEE-6E8BE77D7028}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>